<commit_message>
Changes to show only to Dr. Mubarak saved
</commit_message>
<xml_diff>
--- a/assets/latest data/UVA Gro nutient requirements (3).xlsx
+++ b/assets/latest data/UVA Gro nutient requirements (3).xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="44">
   <si>
     <t>bodyweight</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>CP required (g)</t>
+  </si>
+  <si>
+    <t>cp % of dmi</t>
   </si>
 </sst>
 </file>
@@ -885,7 +888,9 @@
   </sheetPr>
   <dimension ref="A1:T230"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="69" workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9496,7 +9501,7 @@
   </sheetPr>
   <dimension ref="A1:R163"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="D1" zoomScale="69" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16764,10 +16769,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:G73"/>
+    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16779,7 +16784,7 @@
     <col min="7" max="7" width="13.5703125" style="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16801,8 +16806,11 @@
       <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>300</v>
       </c>
@@ -16825,8 +16833,12 @@
       <c r="G2" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <f>(D2/C2)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>350</v>
       </c>
@@ -16850,7 +16862,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>400</v>
       </c>
@@ -16874,7 +16886,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>450</v>
       </c>
@@ -16898,7 +16910,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>500</v>
       </c>
@@ -16922,7 +16934,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>550</v>
       </c>
@@ -16946,7 +16958,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>600</v>
       </c>
@@ -16970,7 +16982,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>650</v>
       </c>
@@ -16994,7 +17006,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>700</v>
       </c>
@@ -17018,7 +17030,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>300</v>
       </c>
@@ -17042,7 +17054,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>350</v>
       </c>
@@ -17066,7 +17078,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>400</v>
       </c>
@@ -17090,7 +17102,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>450</v>
       </c>
@@ -17114,7 +17126,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>500</v>
       </c>
@@ -17138,7 +17150,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>550</v>
       </c>

</xml_diff>